<commit_message>
sporta match excel export + better match frenoy sync
</commit_message>
<xml_diff>
--- a/src/Ttc.DataAccess/Resources/SportaScoresheetTemplate.xlsx
+++ b/src/Ttc.DataAccess/Resources/SportaScoresheetTemplate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wouter\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wouter\Dropbox\Personal\Programming\UnixCode\ttc\react-redux\backend\src\Ttc.WebApi\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A71A81CC-775E-48FF-A9EB-D8996A975F38}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{857F1934-53BE-476B-84D7-21E9DDE17893}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="12120" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1042,183 +1042,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1236,6 +1059,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1246,18 +1072,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1266,6 +1112,160 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2052,7 +2052,7 @@
   <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2072,15 +2072,15 @@
       <c r="A1" s="11"/>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
-      <c r="D1" s="113" t="s">
+      <c r="D1" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
@@ -2089,42 +2089,42 @@
       <c r="P1" s="11"/>
       <c r="Q1" s="11"/>
       <c r="R1" s="11"/>
-      <c r="S1" s="126" t="s">
+      <c r="S1" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
+      <c r="T1" s="74"/>
+      <c r="U1" s="74"/>
+      <c r="V1" s="74"/>
+      <c r="W1" s="74"/>
     </row>
     <row r="2" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
-      <c r="D2" s="113" t="s">
+      <c r="D2" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="90"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
-      <c r="M2" s="105" t="s">
+      <c r="M2" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="N2" s="105"/>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
-      <c r="U2" s="105"/>
-      <c r="V2" s="105"/>
-      <c r="W2" s="105"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
     </row>
     <row r="3" spans="1:25" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
@@ -2132,44 +2132,44 @@
       <c r="C3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="E3" s="113"/>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="113"/>
-      <c r="I3" s="113"/>
-      <c r="J3" s="113"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
       <c r="P3" s="11"/>
-      <c r="Q3" s="113" t="s">
+      <c r="Q3" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="R3" s="113"/>
-      <c r="S3" s="113"/>
-      <c r="T3" s="94" t="s">
+      <c r="R3" s="90"/>
+      <c r="S3" s="90"/>
+      <c r="T3" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="94"/>
-      <c r="V3" s="94"/>
-      <c r="W3" s="94"/>
+      <c r="U3" s="110"/>
+      <c r="V3" s="110"/>
+      <c r="W3" s="110"/>
     </row>
     <row r="4" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="95" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="109"/>
-      <c r="D4" s="109"/>
-      <c r="E4" s="109"/>
-      <c r="F4" s="109"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="15"/>
@@ -2180,26 +2180,26 @@
       <c r="N4" s="16"/>
       <c r="O4" s="16"/>
       <c r="P4" s="16"/>
-      <c r="Q4" s="80" t="s">
+      <c r="Q4" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="R4" s="93"/>
-      <c r="S4" s="93"/>
-      <c r="T4" s="93"/>
-      <c r="U4" s="130"/>
-      <c r="V4" s="130"/>
-      <c r="W4" s="130"/>
+      <c r="R4" s="109"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="109"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
     </row>
     <row r="5" spans="1:25" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
-      <c r="B5" s="108" t="str">
+      <c r="B5" s="94" t="str">
         <f>IF(B4="TTC Erembodegem","Groeneweg 28 - 9320 Erembodegem",IF(B4="De Eekhoorn","Brusselbaan 255 - 9320 Erembodegem",""))</f>
         <v>Groeneweg 28 - 9320 Erembodegem</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="15"/>
@@ -2210,16 +2210,16 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="65" t="s">
+      <c r="Q5" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65" t="s">
+      <c r="R5" s="113"/>
+      <c r="S5" s="113"/>
+      <c r="T5" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
+      <c r="U5" s="113"/>
+      <c r="V5" s="113"/>
       <c r="W5" s="55"/>
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
@@ -2228,17 +2228,17 @@
       <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
+      <c r="B6" s="130"/>
+      <c r="C6" s="130"/>
       <c r="D6" s="63" t="s">
         <v>119</v>
       </c>
       <c r="E6" s="62"/>
       <c r="F6" s="62"/>
-      <c r="G6" s="76" t="s">
+      <c r="G6" s="135" t="s">
         <v>120</v>
       </c>
-      <c r="H6" s="76"/>
+      <c r="H6" s="135"/>
       <c r="I6" s="19"/>
       <c r="J6" s="11"/>
       <c r="K6" s="19"/>
@@ -2281,18 +2281,18 @@
       <c r="W7" s="11"/>
     </row>
     <row r="8" spans="1:25" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="68"/>
+      <c r="B8" s="101"/>
+      <c r="C8" s="102"/>
       <c r="D8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="80" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="23" t="s">
@@ -2302,46 +2302,46 @@
         <v>10</v>
       </c>
       <c r="I8" s="11"/>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="75" t="s">
+      <c r="L8" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="127" t="s">
+      <c r="M8" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="N8" s="128"/>
-      <c r="O8" s="131" t="s">
+      <c r="N8" s="76"/>
+      <c r="O8" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131"/>
-      <c r="S8" s="132"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="82"/>
       <c r="T8" s="26"/>
       <c r="U8" s="27"/>
       <c r="V8" s="27"/>
       <c r="W8" s="28"/>
     </row>
     <row r="9" spans="1:25" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="74"/>
+      <c r="A9" s="132"/>
+      <c r="B9" s="133"/>
+      <c r="C9" s="134"/>
       <c r="D9" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
       <c r="G9" s="30"/>
       <c r="H9" s="31"/>
       <c r="I9" s="15"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
       <c r="M9" s="32" t="s">
         <v>78</v>
       </c>
@@ -2363,31 +2363,31 @@
       <c r="S9" s="33">
         <v>5</v>
       </c>
-      <c r="T9" s="129" t="s">
+      <c r="T9" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="U9" s="101"/>
-      <c r="V9" s="101" t="s">
+      <c r="U9" s="78"/>
+      <c r="V9" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="W9" s="102"/>
+      <c r="W9" s="115"/>
     </row>
     <row r="10" spans="1:25" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25">
         <v>1</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="71"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="103"/>
       <c r="D10" s="49" t="str">
-        <f>IF(ISERROR(VLOOKUP(B10,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B10,Spelers!A1:E33,4))</f>
+        <f>IF(ISERROR(VLOOKUP(B10,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B10,Spelers!A2:E50,4))</f>
         <v/>
       </c>
       <c r="E10" s="49" t="str">
-        <f>IF(ISERROR(VLOOKUP(B10,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B10,Spelers!A1:E33,3))</f>
+        <f>IF(ISERROR(VLOOKUP(B10,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B10,Spelers!A2:E50,3))</f>
         <v/>
       </c>
       <c r="F10" s="49" t="str">
-        <f>IF(ISERROR(VLOOKUP(B10,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B10,Spelers!A1:E33,2))</f>
+        <f>IF(ISERROR(VLOOKUP(B10,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B10,Spelers!A2:E50,2))</f>
         <v/>
       </c>
       <c r="G10" s="37">
@@ -2436,18 +2436,18 @@
       <c r="A11" s="25">
         <v>2</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="97"/>
       <c r="D11" s="49" t="str">
-        <f>IF(ISERROR(VLOOKUP(B11,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B11,Spelers!A1:E33,4))</f>
+        <f>IF(ISERROR(VLOOKUP(B11,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B11,Spelers!A2:E50,4))</f>
         <v/>
       </c>
       <c r="E11" s="49" t="str">
-        <f>IF(ISERROR(VLOOKUP(B11,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B11,Spelers!A1:E33,3))</f>
+        <f>IF(ISERROR(VLOOKUP(B11,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B11,Spelers!A2:E50,3))</f>
         <v/>
       </c>
       <c r="F11" s="49" t="str">
-        <f>IF(ISERROR(VLOOKUP(B11,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B11,Spelers!A1:E33,2))</f>
+        <f>IF(ISERROR(VLOOKUP(B11,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B11,Spelers!A2:E50,2))</f>
         <v/>
       </c>
       <c r="G11" s="37">
@@ -2496,18 +2496,18 @@
       <c r="A12" s="25">
         <v>3</v>
       </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
+      <c r="B12" s="131"/>
+      <c r="C12" s="97"/>
       <c r="D12" s="25" t="str">
-        <f>IF(ISERROR(VLOOKUP(B12,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B12,Spelers!A1:E33,4))</f>
+        <f>IF(ISERROR(VLOOKUP(B12,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B12,Spelers!A2:E50,4))</f>
         <v/>
       </c>
       <c r="E12" s="25" t="str">
-        <f>IF(ISERROR(VLOOKUP(B12,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B12,Spelers!A1:E33,3))</f>
+        <f>IF(ISERROR(VLOOKUP(B12,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B12,Spelers!A2:E50,3))</f>
         <v/>
       </c>
       <c r="F12" s="25" t="str">
-        <f>IF(ISERROR(VLOOKUP(B12,Spelers!A1:E33,4))=TRUE,"",VLOOKUP(B12,Spelers!A1:E33,2))</f>
+        <f>IF(ISERROR(VLOOKUP(B12,Spelers!A2:E50,4))=TRUE,"",VLOOKUP(B12,Spelers!A2:E50,2))</f>
         <v/>
       </c>
       <c r="G12" s="37">
@@ -2556,10 +2556,10 @@
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="106" t="s">
+      <c r="D13" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="107"/>
+      <c r="E13" s="93"/>
       <c r="F13" s="41">
         <f>SUM(F10:F12)</f>
         <v>0</v>
@@ -2644,20 +2644,20 @@
       </c>
     </row>
     <row r="15" spans="1:25" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="67"/>
-      <c r="C15" s="68" t="s">
+      <c r="B15" s="101"/>
+      <c r="C15" s="102" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="80" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="23" t="s">
@@ -2701,81 +2701,81 @@
       </c>
     </row>
     <row r="16" spans="1:25" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="117"/>
-      <c r="B16" s="118"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="123" t="s">
+      <c r="A16" s="64"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="125"/>
-      <c r="H16" s="125"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="111">
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="107"/>
+      <c r="J16" s="98">
         <v>7</v>
       </c>
-      <c r="K16" s="133" t="s">
+      <c r="K16" s="87" t="s">
         <v>79</v>
       </c>
-      <c r="L16" s="134"/>
-      <c r="M16" s="134"/>
-      <c r="N16" s="135"/>
-      <c r="O16" s="95"/>
-      <c r="P16" s="95"/>
-      <c r="Q16" s="95"/>
-      <c r="R16" s="95"/>
-      <c r="S16" s="95"/>
-      <c r="T16" s="103">
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
+      <c r="N16" s="89"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="83"/>
+      <c r="Q16" s="83"/>
+      <c r="R16" s="83"/>
+      <c r="S16" s="83"/>
+      <c r="T16" s="85">
         <f>hulpvariabelen!I9+hulpvariabelen!R9+hulpvariabelen!AA9+hulpvariabelen!AJ9+hulpvariabelen!AS9</f>
         <v>0</v>
       </c>
-      <c r="U16" s="103">
+      <c r="U16" s="85">
         <f>hulpvariabelen!J9+hulpvariabelen!S9+hulpvariabelen!AB9+hulpvariabelen!AK9+hulpvariabelen!AT9</f>
         <v>0</v>
       </c>
-      <c r="V16" s="99" t="str">
+      <c r="V16" s="114" t="str">
         <f>IF(T16=3,"X","")</f>
         <v/>
       </c>
-      <c r="W16" s="99" t="str">
+      <c r="W16" s="114" t="str">
         <f>IF(U16=3,"X","")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:27" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="120"/>
-      <c r="B17" s="121"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="124"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="100"/>
-      <c r="I17" s="86"/>
-      <c r="J17" s="112"/>
-      <c r="K17" s="114" t="s">
+      <c r="A17" s="67"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="107"/>
+      <c r="J17" s="99"/>
+      <c r="K17" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="L17" s="115"/>
-      <c r="M17" s="115"/>
-      <c r="N17" s="116"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
-      <c r="R17" s="96"/>
-      <c r="S17" s="96"/>
-      <c r="T17" s="104"/>
-      <c r="U17" s="104"/>
-      <c r="V17" s="100"/>
-      <c r="W17" s="100"/>
+      <c r="L17" s="105"/>
+      <c r="M17" s="105"/>
+      <c r="N17" s="106"/>
+      <c r="O17" s="84"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="84"/>
+      <c r="R17" s="84"/>
+      <c r="S17" s="84"/>
+      <c r="T17" s="86"/>
+      <c r="U17" s="86"/>
+      <c r="V17" s="73"/>
+      <c r="W17" s="73"/>
     </row>
     <row r="18" spans="1:27" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25">
         <v>1</v>
       </c>
-      <c r="B18" s="110"/>
-      <c r="C18" s="71"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="103"/>
       <c r="D18" s="25"/>
       <c r="E18" s="56"/>
       <c r="F18" s="25"/>
@@ -2825,8 +2825,8 @@
       <c r="A19" s="25">
         <v>2</v>
       </c>
-      <c r="B19" s="110"/>
-      <c r="C19" s="70"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="97"/>
       <c r="D19" s="25"/>
       <c r="E19" s="56"/>
       <c r="F19" s="25"/>
@@ -2876,8 +2876,8 @@
       <c r="A20" s="25">
         <v>3</v>
       </c>
-      <c r="B20" s="110"/>
-      <c r="C20" s="70"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
       <c r="D20" s="25"/>
       <c r="E20" s="56"/>
       <c r="F20" s="25"/>
@@ -2927,10 +2927,10 @@
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
-      <c r="D21" s="106" t="s">
+      <c r="D21" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="107"/>
+      <c r="E21" s="93"/>
       <c r="F21" s="41">
         <f>SUM(F18:F20)</f>
         <v>0</v>
@@ -2946,10 +2946,10 @@
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
       <c r="Q21" s="11"/>
-      <c r="R21" s="97" t="s">
+      <c r="R21" s="111" t="s">
         <v>17</v>
       </c>
-      <c r="S21" s="98"/>
+      <c r="S21" s="112"/>
       <c r="T21" s="34">
         <f>SUM(T10:T20)</f>
         <v>0</v>
@@ -2994,168 +2994,168 @@
       <c r="AA22" s="2"/>
     </row>
     <row r="23" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="80" t="s">
+      <c r="A23" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="80"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="81"/>
-      <c r="J23" s="81"/>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="81"/>
-      <c r="O23" s="81"/>
-      <c r="P23" s="81"/>
-      <c r="Q23" s="81"/>
-      <c r="R23" s="81"/>
-      <c r="S23" s="81"/>
-      <c r="T23" s="81"/>
-      <c r="U23" s="81"/>
-      <c r="V23" s="81"/>
-      <c r="W23" s="81"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="108"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
+      <c r="G23" s="119"/>
+      <c r="H23" s="119"/>
+      <c r="I23" s="119"/>
+      <c r="J23" s="119"/>
+      <c r="K23" s="119"/>
+      <c r="L23" s="119"/>
+      <c r="M23" s="119"/>
+      <c r="N23" s="119"/>
+      <c r="O23" s="119"/>
+      <c r="P23" s="119"/>
+      <c r="Q23" s="119"/>
+      <c r="R23" s="119"/>
+      <c r="S23" s="119"/>
+      <c r="T23" s="119"/>
+      <c r="U23" s="119"/>
+      <c r="V23" s="119"/>
+      <c r="W23" s="119"/>
     </row>
     <row r="24" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="82"/>
-      <c r="B24" s="82"/>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
-      <c r="G24" s="83"/>
-      <c r="H24" s="83"/>
-      <c r="I24" s="83"/>
-      <c r="J24" s="83"/>
-      <c r="K24" s="83"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="83"/>
-      <c r="N24" s="83"/>
-      <c r="O24" s="83"/>
-      <c r="P24" s="83"/>
-      <c r="Q24" s="83"/>
-      <c r="R24" s="83"/>
-      <c r="S24" s="83"/>
-      <c r="T24" s="83"/>
-      <c r="U24" s="83"/>
-      <c r="V24" s="83"/>
-      <c r="W24" s="83"/>
+      <c r="A24" s="120"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="121"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="121"/>
+      <c r="H24" s="121"/>
+      <c r="I24" s="121"/>
+      <c r="J24" s="121"/>
+      <c r="K24" s="121"/>
+      <c r="L24" s="121"/>
+      <c r="M24" s="121"/>
+      <c r="N24" s="121"/>
+      <c r="O24" s="121"/>
+      <c r="P24" s="121"/>
+      <c r="Q24" s="121"/>
+      <c r="R24" s="121"/>
+      <c r="S24" s="121"/>
+      <c r="T24" s="121"/>
+      <c r="U24" s="121"/>
+      <c r="V24" s="121"/>
+      <c r="W24" s="121"/>
     </row>
     <row r="25" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="90"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="90"/>
-      <c r="G25" s="90"/>
-      <c r="H25" s="90"/>
-      <c r="I25" s="90"/>
-      <c r="J25" s="90"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="90"/>
-      <c r="N25" s="90"/>
-      <c r="O25" s="90"/>
-      <c r="P25" s="90"/>
-      <c r="Q25" s="90"/>
-      <c r="R25" s="90"/>
-      <c r="S25" s="90"/>
-      <c r="T25" s="90"/>
-      <c r="U25" s="90"/>
-      <c r="V25" s="90"/>
-      <c r="W25" s="90"/>
+      <c r="A25" s="127"/>
+      <c r="B25" s="127"/>
+      <c r="C25" s="127"/>
+      <c r="D25" s="127"/>
+      <c r="E25" s="127"/>
+      <c r="F25" s="127"/>
+      <c r="G25" s="127"/>
+      <c r="H25" s="127"/>
+      <c r="I25" s="127"/>
+      <c r="J25" s="127"/>
+      <c r="K25" s="127"/>
+      <c r="L25" s="127"/>
+      <c r="M25" s="127"/>
+      <c r="N25" s="127"/>
+      <c r="O25" s="127"/>
+      <c r="P25" s="127"/>
+      <c r="Q25" s="127"/>
+      <c r="R25" s="127"/>
+      <c r="S25" s="127"/>
+      <c r="T25" s="127"/>
+      <c r="U25" s="127"/>
+      <c r="V25" s="127"/>
+      <c r="W25" s="127"/>
     </row>
     <row r="26" spans="1:27" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="128" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128"/>
+      <c r="F26" s="128"/>
+      <c r="G26" s="128"/>
       <c r="H26" s="11"/>
       <c r="I26" s="11"/>
       <c r="J26" s="11"/>
       <c r="K26" s="11"/>
       <c r="L26" s="11"/>
-      <c r="M26" s="92" t="s">
+      <c r="M26" s="129" t="s">
         <v>41</v>
       </c>
-      <c r="N26" s="92"/>
-      <c r="O26" s="92"/>
-      <c r="P26" s="92"/>
-      <c r="Q26" s="92"/>
-      <c r="R26" s="92"/>
-      <c r="S26" s="92"/>
-      <c r="T26" s="92"/>
-      <c r="U26" s="92"/>
-      <c r="V26" s="92"/>
-      <c r="W26" s="92"/>
+      <c r="N26" s="129"/>
+      <c r="O26" s="129"/>
+      <c r="P26" s="129"/>
+      <c r="Q26" s="129"/>
+      <c r="R26" s="129"/>
+      <c r="S26" s="129"/>
+      <c r="T26" s="129"/>
+      <c r="U26" s="129"/>
+      <c r="V26" s="129"/>
+      <c r="W26" s="129"/>
     </row>
     <row r="27" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="84"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
+      <c r="A27" s="122"/>
+      <c r="B27" s="122"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="122"/>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
-      <c r="H27" s="77" t="s">
+      <c r="H27" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="78"/>
-      <c r="J27" s="78"/>
-      <c r="K27" s="78"/>
-      <c r="L27" s="79"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="118"/>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
-      <c r="P27" s="86"/>
-      <c r="Q27" s="86"/>
-      <c r="R27" s="86"/>
-      <c r="S27" s="86"/>
-      <c r="T27" s="86"/>
-      <c r="U27" s="86"/>
-      <c r="V27" s="86"/>
-      <c r="W27" s="86"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
+      <c r="S27" s="107"/>
+      <c r="T27" s="107"/>
+      <c r="U27" s="107"/>
+      <c r="V27" s="107"/>
+      <c r="W27" s="107"/>
     </row>
     <row r="28" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="84"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
+      <c r="A28" s="122"/>
+      <c r="B28" s="122"/>
+      <c r="C28" s="122"/>
+      <c r="D28" s="122"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
       <c r="G28" s="11"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="88"/>
-      <c r="J28" s="88"/>
-      <c r="K28" s="88"/>
-      <c r="L28" s="89"/>
+      <c r="H28" s="124"/>
+      <c r="I28" s="125"/>
+      <c r="J28" s="125"/>
+      <c r="K28" s="125"/>
+      <c r="L28" s="126"/>
       <c r="M28" s="11"/>
       <c r="N28" s="11"/>
       <c r="O28" s="11"/>
-      <c r="P28" s="86"/>
-      <c r="Q28" s="86"/>
-      <c r="R28" s="86"/>
-      <c r="S28" s="86"/>
-      <c r="T28" s="86"/>
-      <c r="U28" s="86"/>
-      <c r="V28" s="86"/>
-      <c r="W28" s="86"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
+      <c r="S28" s="107"/>
+      <c r="T28" s="107"/>
+      <c r="U28" s="107"/>
+      <c r="V28" s="107"/>
+      <c r="W28" s="107"/>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A29" s="85"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="85"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="123"/>
+      <c r="C29" s="123"/>
+      <c r="D29" s="123"/>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
@@ -3167,14 +3167,14 @@
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11"/>
-      <c r="P29" s="85"/>
-      <c r="Q29" s="85"/>
-      <c r="R29" s="85"/>
-      <c r="S29" s="85"/>
-      <c r="T29" s="85"/>
-      <c r="U29" s="85"/>
-      <c r="V29" s="85"/>
-      <c r="W29" s="85"/>
+      <c r="P29" s="123"/>
+      <c r="Q29" s="123"/>
+      <c r="R29" s="123"/>
+      <c r="S29" s="123"/>
+      <c r="T29" s="123"/>
+      <c r="U29" s="123"/>
+      <c r="V29" s="123"/>
+      <c r="W29" s="123"/>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
@@ -3256,6 +3256,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="T5:V5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="H27:L27"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E23:W23"/>
+    <mergeCell ref="A24:W24"/>
+    <mergeCell ref="A27:D29"/>
+    <mergeCell ref="P27:W29"/>
+    <mergeCell ref="H28:L28"/>
+    <mergeCell ref="A25:W25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="M26:W26"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="Q5:S5"/>
+    <mergeCell ref="W16:W17"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="S16:S17"/>
+    <mergeCell ref="V9:W9"/>
+    <mergeCell ref="U16:U17"/>
+    <mergeCell ref="V16:V17"/>
+    <mergeCell ref="M2:W2"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="I16:I17"/>
     <mergeCell ref="A16:C17"/>
     <mergeCell ref="D16:D17"/>
     <mergeCell ref="H16:H17"/>
@@ -3272,55 +3321,6 @@
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="D3:J3"/>
-    <mergeCell ref="M2:W2"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="R21:S21"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="Q5:S5"/>
-    <mergeCell ref="W16:W17"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="S16:S17"/>
-    <mergeCell ref="V9:W9"/>
-    <mergeCell ref="U16:U17"/>
-    <mergeCell ref="V16:V17"/>
-    <mergeCell ref="H27:L27"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E23:W23"/>
-    <mergeCell ref="A24:W24"/>
-    <mergeCell ref="A27:D29"/>
-    <mergeCell ref="P27:W29"/>
-    <mergeCell ref="H28:L28"/>
-    <mergeCell ref="A25:W25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="M26:W26"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="T5:V5"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G6:H6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="K17 U4:W4 A9:C9 B6:C6 C11:C12 H28 B10:B12 A16 B18:C20 D18:F18 D20:F20">
@@ -7224,12 +7224,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="A54:C54"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="A51:C51"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="D45:F45"/>
     <mergeCell ref="A1:C1"/>
@@ -7242,6 +7236,12 @@
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="A42:C42"/>
     <mergeCell ref="D42:F42"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="A51:C51"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>